<commit_message>
Added Algorithm for Aufgabe 3
</commit_message>
<xml_diff>
--- a/Materialien/Aufgabe01/Uebersicht.xlsx
+++ b/Materialien/Aufgabe01/Uebersicht.xlsx
@@ -121,17 +121,17 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -415,42 +415,42 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="4" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5">
@@ -461,66 +461,63 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>115</v>
+        <v>1040</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9">
-        <v>31</v>
-      </c>
       <c r="G9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>